<commit_message>
:art: refactor: edit MerchantServiceImpl and its test and add basic cards to predefined database
</commit_message>
<xml_diff>
--- a/hodgepodge_cards.xlsx
+++ b/hodgepodge_cards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivi\Documents\projektek\hodgepodge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\hodgepodge\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">merchant!$B$1:$B$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">merchant!$B$1:$B$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="171">
   <si>
     <t>RR</t>
   </si>
@@ -590,7 +590,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,14 +627,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -642,42 +636,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -735,17 +698,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,12 +982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1044,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1106,14 +1059,14 @@
         <v>2</v>
       </c>
       <c r="F2" s="4">
-        <f t="shared" ref="F2:F46" si="0">G2*E2</f>
+        <f t="shared" ref="F2:F54" si="0">G2*E2</f>
         <v>2</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
       </c>
       <c r="H2" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
@@ -1125,105 +1078,109 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="17">
-        <v>2</v>
-      </c>
-      <c r="F3" s="6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G3" s="6">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F6" si="1">G3*E3</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>161</v>
+      <c r="H3" s="4">
+        <v>100</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>150</v>
       </c>
       <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="H4" s="4">
+        <v>100</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="21">
-        <f>-3+4</f>
+      <c r="B5" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="F4" s="21">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G4" s="21">
-        <v>3</v>
-      </c>
-      <c r="H4" s="21">
-        <v>3</v>
-      </c>
-      <c r="I4" s="21">
-        <v>31</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="21">
-        <f>-2+3</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="21">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G5" s="21">
-        <v>3</v>
-      </c>
-      <c r="H5" s="21">
-        <v>21</v>
-      </c>
-      <c r="I5" s="21">
-        <v>3</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="4">
+        <v>100</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1232,91 +1189,92 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>130</v>
+        <v>100</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+        <v>150</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="B7" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="17">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>21</v>
+      <c r="H7" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+        <v>150</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="17">
+        <v>2</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" ref="F8:F11" si="2">G8*E8</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="E8" s="4">
-        <v>3</v>
-      </c>
-      <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>3</v>
+      <c r="H8" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1326,11 +1284,11 @@
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="G9" s="6">
         <v>1</v>
@@ -1339,944 +1297,923 @@
         <v>160</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+        <v>150</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="17">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="17">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="21">
-        <f>-6+6+2</f>
-        <v>2</v>
-      </c>
-      <c r="F10" s="21">
-        <f t="shared" si="0"/>
+      <c r="C12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="21">
-        <v>2</v>
-      </c>
-      <c r="H10" s="21">
-        <v>22</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
-        <v>10</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="E12" s="15">
+        <f>-3+4</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G12" s="15">
+        <v>3</v>
+      </c>
+      <c r="H12" s="15">
+        <v>3</v>
+      </c>
+      <c r="I12" s="15">
+        <v>31</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="21">
-        <f>-6+4+2+2</f>
-        <v>2</v>
-      </c>
-      <c r="F11" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G11" s="21">
-        <v>2</v>
-      </c>
-      <c r="H11" s="21">
-        <v>22</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
-        <v>11</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="21">
-        <f>-4+3+3</f>
-        <v>2</v>
-      </c>
-      <c r="F12" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G12" s="21">
-        <v>2</v>
-      </c>
-      <c r="H12" s="21">
-        <v>31</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
-        <v>12</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="21">
-        <f>-4+3+3</f>
-        <v>2</v>
-      </c>
-      <c r="F13" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G13" s="21">
-        <v>2</v>
-      </c>
-      <c r="H13" s="21">
-        <v>12</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="C13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="21">
-        <f>-6+6+2</f>
-        <v>2</v>
-      </c>
-      <c r="F14" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G14" s="21">
-        <v>2</v>
-      </c>
-      <c r="H14" s="21">
-        <v>13</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
-        <v>14</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="21">
-        <f>-4+4+2</f>
-        <v>2</v>
-      </c>
-      <c r="F15" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G15" s="21">
-        <v>2</v>
-      </c>
-      <c r="H15" s="21">
-        <v>31</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
-        <v>15</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="21">
-        <f>-4+6</f>
-        <v>2</v>
-      </c>
-      <c r="F16" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G16" s="21">
-        <v>2</v>
-      </c>
-      <c r="H16" s="21">
-        <v>4</v>
-      </c>
-      <c r="I16" s="21">
-        <v>32</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="4">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="D13" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4">
-        <v>4</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>4</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="4">
-        <v>4</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G19" s="4">
-        <v>1</v>
-      </c>
-      <c r="H19" s="4">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <v>31</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="4">
-        <v>4</v>
-      </c>
-      <c r="F20" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4">
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <v>22</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
-      <c r="H21" s="4">
-        <v>0</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
-        <v>21</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="21">
+      <c r="E13" s="15">
         <f>-2+3</f>
         <v>1</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F13" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G13" s="15">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15">
+        <v>21</v>
+      </c>
+      <c r="I13" s="15">
+        <v>3</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>100</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>100</v>
+      </c>
+      <c r="I15" s="4">
+        <v>21</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>100</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="17">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="15">
+        <f>-6+6+2</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G18" s="15">
+        <v>2</v>
+      </c>
+      <c r="H18" s="15">
+        <v>22</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="15">
+        <f>-6+4+2+2</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G19" s="15">
+        <v>2</v>
+      </c>
+      <c r="H19" s="15">
+        <v>22</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="15">
+        <f>-4+3+3</f>
+        <v>2</v>
+      </c>
+      <c r="F20" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G20" s="15">
+        <v>2</v>
+      </c>
+      <c r="H20" s="15">
+        <v>31</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="15">
+        <f>-4+3+3</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G21" s="15">
+        <v>2</v>
+      </c>
+      <c r="H21" s="15">
+        <v>12</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="15">
+        <f>-6+6+2</f>
+        <v>2</v>
+      </c>
+      <c r="F22" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G22" s="15">
+        <v>2</v>
+      </c>
+      <c r="H22" s="15">
+        <v>13</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="15">
+        <f>-4+4+2</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="15">
+        <v>2</v>
+      </c>
+      <c r="H23" s="15">
+        <v>31</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="15">
+        <f>-4+6</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G24" s="15">
+        <v>2</v>
+      </c>
+      <c r="H24" s="15">
+        <v>4</v>
+      </c>
+      <c r="I24" s="15">
+        <v>32</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="4">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1</v>
+      </c>
+      <c r="H25" s="4">
+        <v>100</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1</v>
+      </c>
+      <c r="H26" s="4">
+        <v>100</v>
+      </c>
+      <c r="I26" s="4">
+        <v>4</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
+      <c r="H27" s="4">
+        <v>100</v>
+      </c>
+      <c r="I27" s="4">
+        <v>31</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1</v>
+      </c>
+      <c r="H28" s="4">
+        <v>100</v>
+      </c>
+      <c r="I28" s="4">
+        <v>22</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4">
+        <v>4</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="H29" s="4">
+        <v>100</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="15">
+        <f>-2+3</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G30" s="15">
         <v>5</v>
       </c>
-      <c r="H22" s="21">
-        <v>2</v>
-      </c>
-      <c r="I22" s="21">
+      <c r="H30" s="15">
+        <v>2</v>
+      </c>
+      <c r="I30" s="15">
         <v>21</v>
       </c>
-      <c r="J22" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
-        <v>22</v>
-      </c>
-      <c r="B23" s="21" t="s">
+      <c r="J30" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>30</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C31" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D31" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E31" s="15">
         <f>-2-1+4</f>
         <v>1</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F31" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G31" s="15">
         <v>5</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H31" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I31" s="15">
         <v>31</v>
       </c>
-      <c r="J23" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
-        <v>23</v>
-      </c>
-      <c r="B24" s="21" t="s">
+      <c r="J31" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E32" s="15">
         <f>-3+4</f>
         <v>1</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F32" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G32" s="15">
         <v>5</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H32" s="15">
         <v>21</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I32" s="15">
         <v>12</v>
       </c>
-      <c r="J24" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21">
-        <v>24</v>
-      </c>
-      <c r="B25" s="21" t="s">
+      <c r="J32" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C33" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D33" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E33" s="15">
         <f>-4+4+2</f>
         <v>2</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F33" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G25" s="21">
-        <v>3</v>
-      </c>
-      <c r="H25" s="21">
+      <c r="G33" s="15">
+        <v>3</v>
+      </c>
+      <c r="H33" s="15">
         <v>12</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I33" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="J25" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
-        <v>25</v>
-      </c>
-      <c r="B26" s="21" t="s">
+      <c r="J33" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>33</v>
+      </c>
+      <c r="B34" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C34" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D34" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E34" s="15">
         <f>-3+2+3</f>
         <v>2</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F34" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G26" s="21">
-        <v>3</v>
-      </c>
-      <c r="H26" s="21">
-        <v>3</v>
-      </c>
-      <c r="I26" s="21" t="s">
+      <c r="G34" s="15">
+        <v>3</v>
+      </c>
+      <c r="H34" s="15">
+        <v>3</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="J26" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21">
-        <v>26</v>
-      </c>
-      <c r="B27" s="21" t="s">
+      <c r="J34" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D35" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E35" s="15">
         <f>-6+4+4</f>
         <v>2</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F35" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G27" s="21">
-        <v>3</v>
-      </c>
-      <c r="H27" s="21">
+      <c r="G35" s="15">
+        <v>3</v>
+      </c>
+      <c r="H35" s="15">
         <v>22</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I35" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="J27" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
-        <v>27</v>
-      </c>
-      <c r="B28" s="21" t="s">
+      <c r="J35" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>35</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D36" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E36" s="15">
         <f>-6+4+3+1</f>
         <v>2</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F36" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G28" s="21">
-        <v>3</v>
-      </c>
-      <c r="H28" s="21">
+      <c r="G36" s="15">
+        <v>3</v>
+      </c>
+      <c r="H36" s="15">
         <v>13</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="I36" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="J28" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23">
-        <v>28</v>
-      </c>
-      <c r="B29" s="23" t="s">
+      <c r="J36" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>36</v>
+      </c>
+      <c r="B37" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C37" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D37" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E37" s="15">
         <f>-4+2+2+2</f>
         <v>2</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F37" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G29" s="21">
-        <v>3</v>
-      </c>
-      <c r="H29" s="21">
+      <c r="G37" s="15">
+        <v>3</v>
+      </c>
+      <c r="H37" s="15">
         <v>31</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I37" s="15">
         <v>13</v>
-      </c>
-      <c r="J29" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="5">
-        <f>-6+8</f>
-        <v>2</v>
-      </c>
-      <c r="F30" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G30" s="5">
-        <v>3</v>
-      </c>
-      <c r="H30" s="5">
-        <v>13</v>
-      </c>
-      <c r="I30" s="5">
-        <v>32</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="5">
-        <f>-4+3+2+1</f>
-        <v>2</v>
-      </c>
-      <c r="F31" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G31" s="5">
-        <v>3</v>
-      </c>
-      <c r="H31" s="5">
-        <v>31</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="5">
-        <f>-3+4+1</f>
-        <v>2</v>
-      </c>
-      <c r="F32" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G32" s="5">
-        <v>3</v>
-      </c>
-      <c r="H32" s="5">
-        <v>21</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J32" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="5">
-        <f>-3+2+4</f>
-        <v>3</v>
-      </c>
-      <c r="F33" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G33" s="5">
-        <v>2</v>
-      </c>
-      <c r="H33" s="5">
-        <v>21</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="5">
-        <f>-5+8</f>
-        <v>3</v>
-      </c>
-      <c r="F34" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G34" s="5">
-        <v>2</v>
-      </c>
-      <c r="H34" s="5">
-        <v>5</v>
-      </c>
-      <c r="I34" s="5">
-        <v>32</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="5">
-        <f>-4+3+4</f>
-        <v>3</v>
-      </c>
-      <c r="F35" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G35" s="5">
-        <v>2</v>
-      </c>
-      <c r="H35" s="5">
-        <v>4</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="5">
-        <f>-4-4+3+3+6</f>
-        <v>4</v>
-      </c>
-      <c r="F36" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G36" s="5">
-        <v>2</v>
-      </c>
-      <c r="H36" s="5">
-        <v>32</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="5">
-        <f>-8+9+2+1</f>
-        <v>4</v>
-      </c>
-      <c r="F37" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G37" s="5">
-        <v>2</v>
-      </c>
-      <c r="H37" s="5">
-        <v>32</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="J37" s="15" t="s">
         <v>152</v>
@@ -2290,27 +2227,27 @@
         <v>170</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E38" s="5">
-        <f>-5+9</f>
-        <v>4</v>
+        <f>-6+8</f>
+        <v>2</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G38" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H38" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I38" s="5">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J38" s="15" t="s">
         <v>152</v>
@@ -2324,27 +2261,27 @@
         <v>170</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="5">
+        <f>-4+3+2+1</f>
+        <v>2</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E39" s="5">
-        <f>-3-2+4+4</f>
-        <v>3</v>
-      </c>
-      <c r="F39" s="5">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="G39" s="5">
         <v>3</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I39" s="5">
-        <v>32</v>
+      <c r="H39" s="5">
+        <v>31</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="J39" s="15" t="s">
         <v>152</v>
@@ -2358,27 +2295,27 @@
         <v>170</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E40" s="5">
-        <f>-9+4+4+4</f>
-        <v>3</v>
+        <f>-3+4+1</f>
+        <v>2</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G40" s="5">
         <v>3</v>
       </c>
       <c r="H40" s="5">
-        <v>23</v>
-      </c>
-      <c r="I40" s="5">
-        <v>33</v>
+        <v>21</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="J40" s="15" t="s">
         <v>152</v>
@@ -2392,27 +2329,27 @@
         <v>170</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E41" s="5">
-        <f>-6+9</f>
+        <f>-3+2+4</f>
         <v>3</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G41" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H41" s="5">
-        <v>13</v>
-      </c>
-      <c r="I41" s="5">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="J41" s="15" t="s">
         <v>152</v>
@@ -2426,27 +2363,27 @@
         <v>170</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E42" s="5">
-        <f>-3+6</f>
+        <f>-5+8</f>
         <v>3</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G42" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H42" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I42" s="5">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J42" s="15" t="s">
         <v>152</v>
@@ -2460,27 +2397,27 @@
         <v>170</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E43" s="5">
-        <f>-2+4</f>
-        <v>2</v>
+        <f>-4+3+4</f>
+        <v>3</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G43" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H43" s="5">
-        <v>2</v>
-      </c>
-      <c r="I43" s="5">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="J43" s="15" t="s">
         <v>152</v>
@@ -2494,27 +2431,27 @@
         <v>170</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E44" s="5">
-        <f>-6+8</f>
-        <v>2</v>
+        <f>-4-4+3+3+6</f>
+        <v>4</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G44" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H44" s="5">
-        <v>22</v>
-      </c>
-      <c r="I44" s="5">
         <v>32</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="J44" s="15" t="s">
         <v>152</v>
@@ -2528,27 +2465,27 @@
         <v>170</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E45" s="5">
-        <f>-4+6</f>
-        <v>2</v>
+        <f>-8+9+2+1</f>
+        <v>4</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G45" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H45" s="5">
-        <v>12</v>
-      </c>
-      <c r="I45" s="5">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>152</v>
@@ -2562,40 +2499,306 @@
         <v>170</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="5">
+        <f>-5+9</f>
         <v>4</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="F46" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G46" s="5">
+        <v>2</v>
+      </c>
+      <c r="H46" s="5">
+        <v>5</v>
+      </c>
+      <c r="I46" s="5">
+        <v>23</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="5">
+        <f>-3-2+4+4</f>
+        <v>3</v>
+      </c>
+      <c r="F47" s="5">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E46" s="5">
+      <c r="G47" s="5">
+        <v>3</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" s="5">
+        <v>32</v>
+      </c>
+      <c r="J47" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="5">
+        <f>-9+4+4+4</f>
+        <v>3</v>
+      </c>
+      <c r="F48" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G48" s="5">
+        <v>3</v>
+      </c>
+      <c r="H48" s="5">
+        <v>23</v>
+      </c>
+      <c r="I48" s="5">
+        <v>33</v>
+      </c>
+      <c r="J48" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="5">
+        <f>-6+9</f>
+        <v>3</v>
+      </c>
+      <c r="F49" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G49" s="5">
+        <v>3</v>
+      </c>
+      <c r="H49" s="5">
+        <v>13</v>
+      </c>
+      <c r="I49" s="5">
+        <v>23</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="5">
+        <f>-3+6</f>
+        <v>3</v>
+      </c>
+      <c r="F50" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G50" s="5">
+        <v>3</v>
+      </c>
+      <c r="H50" s="5">
+        <v>3</v>
+      </c>
+      <c r="I50" s="5">
+        <v>13</v>
+      </c>
+      <c r="J50" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="5">
+        <f>-2+4</f>
+        <v>2</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G51" s="5">
+        <v>5</v>
+      </c>
+      <c r="H51" s="5">
+        <v>2</v>
+      </c>
+      <c r="I51" s="5">
+        <v>12</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="5">
+        <f>-6+8</f>
+        <v>2</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G52" s="5">
+        <v>5</v>
+      </c>
+      <c r="H52" s="5">
+        <v>22</v>
+      </c>
+      <c r="I52" s="5">
+        <v>32</v>
+      </c>
+      <c r="J52" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="5">
         <f>-4+6</f>
         <v>2</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F53" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G53" s="5">
         <v>5</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H53" s="5">
+        <v>12</v>
+      </c>
+      <c r="I53" s="5">
+        <v>22</v>
+      </c>
+      <c r="J53" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="5">
+        <f>-4+6</f>
+        <v>2</v>
+      </c>
+      <c r="F54" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G54" s="5">
+        <v>5</v>
+      </c>
+      <c r="H54" s="5">
         <v>31</v>
       </c>
-      <c r="I46" s="5">
+      <c r="I54" s="5">
         <v>22</v>
       </c>
-      <c r="J46" s="15" t="s">
+      <c r="J54" s="15" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B46">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="trade"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:B54"/>
   <sortState ref="B2:G46">
     <sortCondition ref="F2:F46"/>
     <sortCondition ref="E2:E46"/>
@@ -2612,7 +2815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,13 +3548,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="13" bestFit="1" customWidth="1"/>
@@ -3820,7 +4023,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="14">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="C42" s="14">
         <v>0</v>

</xml_diff>